<commit_message>
adicion de archivos y actualizaciones
</commit_message>
<xml_diff>
--- a/CoordenadasUTM.xlsx
+++ b/CoordenadasUTM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monse\OneDrive\Pictures\Documents\IA\4to semestre\Fundamentos de IA\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE91B3-CFA1-4505-BBBE-E720AC6F5C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2966BDB-F45B-45AB-A1EC-47E596B7ABED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D319DFB0-5488-483C-AB12-F69BE80286E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Tlaxcala</t>
   </si>
@@ -53,33 +54,12 @@
     <t>Nopalucan</t>
   </si>
   <si>
-    <t>Tlaxcala (cabecera municipal)</t>
-  </si>
-  <si>
-    <t>San Esteban Tizatlán</t>
-  </si>
-  <si>
     <t>San Lucas Cuauhtelulpan</t>
   </si>
   <si>
-    <t>San José Tetel</t>
-  </si>
-  <si>
-    <t>La Loma Xicohténcatl</t>
-  </si>
-  <si>
-    <t>Ocotlán</t>
-  </si>
-  <si>
-    <t>La Joya</t>
-  </si>
-  <si>
     <t>San Gabriel Cuauhtla</t>
   </si>
   <si>
-    <t>Chiautempan (cabecera municipal)</t>
-  </si>
-  <si>
     <t>Santa Ana Chiautempan</t>
   </si>
   <si>
@@ -101,9 +81,6 @@
     <t>San Isidro Buen Suceso</t>
   </si>
   <si>
-    <t>Ixtacuixtla de Mariano Matamoros (cabecera municipal)</t>
-  </si>
-  <si>
     <t>San Pedro Ixtacuixtla</t>
   </si>
   <si>
@@ -122,9 +99,6 @@
     <t>San Lucas Texmelucan</t>
   </si>
   <si>
-    <t>Panotla (cabecera municipal)</t>
-  </si>
-  <si>
     <t>Santa María Panotla</t>
   </si>
   <si>
@@ -146,15 +120,9 @@
     <t>San Francisco Tlacuilohcan</t>
   </si>
   <si>
-    <t>Santa Cruz Nopalucan (cabecera municipal)</t>
-  </si>
-  <si>
     <t>San Lorenzo Axocomanitla</t>
   </si>
   <si>
-    <t>San Martín Texmelucan</t>
-  </si>
-  <si>
     <t>San Sebastián Atlahapa</t>
   </si>
   <si>
@@ -177,6 +145,63 @@
   </si>
   <si>
     <t>NombreLugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiautempan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ixtacuixtla de Mariano Matamoros </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panotla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Cruz Nopalucan </t>
+  </si>
+  <si>
+    <t>San Pablo del Monte</t>
+  </si>
+  <si>
+    <t>Trebol</t>
+  </si>
+  <si>
+    <t>Esc. Prim Xicohtencatl</t>
+  </si>
+  <si>
+    <t>Centro de San Jorge Tezoquipan</t>
+  </si>
+  <si>
+    <t>Entronque Entrada Techachalco</t>
+  </si>
+  <si>
+    <t>Entrada Panotla</t>
+  </si>
+  <si>
+    <t>Iglesia Trinidad Tenexyecac</t>
+  </si>
+  <si>
+    <t>San Jorge Tezoquipan Iglesia</t>
+  </si>
+  <si>
+    <t>Centro Santa Catarina Apatlahco</t>
+  </si>
+  <si>
+    <t>Gasolinera Zaragoza</t>
+  </si>
+  <si>
+    <t>Colegio Tepochcalli</t>
+  </si>
+  <si>
+    <t>Presidencia Auxiliar Xochimilco</t>
+  </si>
+  <si>
+    <t>Ixtacuixtla de Mariano Matamoros</t>
+  </si>
+  <si>
+    <t>Mercado municipal Emilio Sanchez Piedras</t>
+  </si>
+  <si>
+    <t>Escuela Normal Preescolar PFMM</t>
   </si>
 </sst>
 </file>
@@ -558,29 +583,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439DFE7B-9C19-4698-887A-2ECBF1529337}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -588,13 +616,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C2">
-        <v>580000</v>
+        <v>579662.41</v>
       </c>
       <c r="D2">
-        <v>2130000</v>
+        <v>2135635.15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -602,543 +630,629 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C3">
-        <v>583000</v>
+        <v>580185.22</v>
       </c>
       <c r="D3">
-        <v>2130500</v>
+        <v>2136201.8199999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C4">
-        <v>579000</v>
+        <v>580870.22</v>
       </c>
       <c r="D4">
-        <v>2130500</v>
+        <v>2138086.1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>582000</v>
+        <v>581846.39</v>
       </c>
       <c r="D5">
-        <v>2131000</v>
+        <v>2138256.4700000002</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C6">
-        <v>580500</v>
+        <v>578501.6</v>
       </c>
       <c r="D6">
-        <v>2130700</v>
+        <v>2139259.7999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>580500</v>
+        <v>578066.09</v>
       </c>
       <c r="D7">
-        <v>2129800</v>
+        <v>2135495.44</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>580500</v>
+        <v>577682.44999999995</v>
       </c>
       <c r="D8">
-        <v>2130200</v>
+        <v>2139223.08</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>580000</v>
+        <v>584158.84</v>
       </c>
       <c r="D9">
-        <v>2129900</v>
+        <v>2135677.52</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C10">
-        <v>584000</v>
+        <v>581614.5</v>
       </c>
       <c r="D10">
-        <v>2131000</v>
+        <v>2138432.48</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>577638.49</v>
+      </c>
+      <c r="D11">
+        <v>2139676.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>578009.35</v>
+      </c>
+      <c r="D12">
+        <v>2138925.69</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>577235.02</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2138225.2200000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>579411.31000000006</v>
+      </c>
+      <c r="D14">
+        <v>2140204.38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A970AFA-F769-4D5D-9A4F-C89FED6B9C0B}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1">
+        <v>580000</v>
+      </c>
+      <c r="D1">
+        <v>2129900</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2">
+        <v>584000</v>
+      </c>
+      <c r="D2">
+        <v>2131000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>585000</v>
+      </c>
+      <c r="D3">
+        <v>2131000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>583000</v>
+      </c>
+      <c r="D4">
+        <v>2131500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>587000</v>
+      </c>
+      <c r="D5">
+        <v>2130700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>587500</v>
+      </c>
+      <c r="D6">
+        <v>2131500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>583500</v>
+      </c>
+      <c r="D7">
+        <v>2130500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>585500</v>
+      </c>
+      <c r="D8">
+        <v>2132000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>585500</v>
+      </c>
+      <c r="D9">
+        <v>2130700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>589000</v>
+      </c>
+      <c r="D10">
+        <v>2130000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>585000</v>
+        <v>588000</v>
       </c>
       <c r="D11">
-        <v>2131000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2130500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12">
-        <v>583000</v>
+        <v>591000</v>
       </c>
       <c r="D12">
-        <v>2131500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2130000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13">
-        <v>587000</v>
+        <v>589500</v>
       </c>
       <c r="D13">
-        <v>2130700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2130500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14">
-        <v>587500</v>
+        <v>591500</v>
       </c>
       <c r="D14">
-        <v>2131500</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2129500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15">
-        <v>583500</v>
+        <v>592000</v>
       </c>
       <c r="D15">
-        <v>2130500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2129000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>585500</v>
+        <v>589000</v>
       </c>
       <c r="D16">
-        <v>2132000</v>
+        <v>2128500</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>585500</v>
+        <v>589500</v>
       </c>
       <c r="D17">
-        <v>2130700</v>
+        <v>2128000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>589000</v>
+        <v>590000</v>
       </c>
       <c r="D18">
-        <v>2130000</v>
+        <v>2128000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19">
-        <v>588000</v>
+        <v>590000</v>
       </c>
       <c r="D19">
-        <v>2130500</v>
+        <v>2128500</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>591000</v>
       </c>
       <c r="D20">
-        <v>2130000</v>
+        <v>2127500</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>589500</v>
       </c>
       <c r="D21">
-        <v>2130500</v>
+        <v>2128500</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22">
-        <v>591500</v>
+        <v>590500</v>
       </c>
       <c r="D22">
-        <v>2129500</v>
+        <v>2129000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>592000</v>
+        <v>588500</v>
       </c>
       <c r="D23">
-        <v>2129000</v>
+        <v>2127500</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>589000</v>
+        <v>590500</v>
       </c>
       <c r="D24">
-        <v>2128500</v>
+        <v>2128000</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>589500</v>
       </c>
       <c r="D25">
-        <v>2128000</v>
+        <v>2127000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C26">
-        <v>590000</v>
+        <v>585000</v>
       </c>
       <c r="D26">
-        <v>2128000</v>
+        <v>2127500</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>590000</v>
+        <v>582000</v>
       </c>
       <c r="D27">
-        <v>2128500</v>
+        <v>2128000</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C28">
-        <v>591000</v>
+        <v>586500</v>
       </c>
       <c r="D28">
-        <v>2127500</v>
+        <v>2127000</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C29">
-        <v>589500</v>
+        <v>587500</v>
       </c>
       <c r="D29">
-        <v>2128500</v>
+        <v>2127500</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C30">
-        <v>590500</v>
+        <v>585500</v>
       </c>
       <c r="D30">
-        <v>2129000</v>
+        <v>2127000</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>588500</v>
+        <v>586500</v>
       </c>
       <c r="D31">
-        <v>2127500</v>
+        <v>2126500</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>590500</v>
-      </c>
-      <c r="D32">
-        <v>2128000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33">
-        <v>589500</v>
-      </c>
-      <c r="D33">
-        <v>2127000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34">
-        <v>585000</v>
-      </c>
-      <c r="D34">
-        <v>2127500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35">
-        <v>582000</v>
-      </c>
-      <c r="D35">
-        <v>2128000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36">
-        <v>586500</v>
-      </c>
-      <c r="D36">
-        <v>2127000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37">
-        <v>584500</v>
-      </c>
-      <c r="D37">
-        <v>2126500</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38">
-        <v>587500</v>
-      </c>
-      <c r="D38">
-        <v>2127500</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39">
-        <v>585500</v>
-      </c>
-      <c r="D39">
-        <v>2127000</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40">
-        <v>586500</v>
-      </c>
-      <c r="D40">
-        <v>2126500</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41">
         <v>584500</v>
       </c>
     </row>

</xml_diff>